<commit_message>
Added qualifiers for determining what bands need to be made
</commit_message>
<xml_diff>
--- a/resources/field_forms/field_form_treereplace[2019].xlsx
+++ b/resources/field_forms/field_form_treereplace[2019].xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgregori\Dropbox (Smithsonian)\Github_Ian\Dendrobands\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgregori\Dropbox (Smithsonian)\Github_Ian\Dendrobands\resources\field_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,17 +13,19 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$68</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="34">
   <si>
     <t>New Dendroband Trees                    Date:                       Surveyors:</t>
   </si>
@@ -114,13 +116,33 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>Band made?</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>dbh cm</t>
+  </si>
+  <si>
+    <t>band length</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -172,17 +194,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,80 +507,90 @@
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
     <col min="8" max="8" width="7.140625" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="15" max="15" width="32" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>30560</v>
       </c>
@@ -570,7 +609,8 @@
       <c r="F3" s="2">
         <v>15.3</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
+        <f>R3*10</f>
         <v>384</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -597,8 +637,18 @@
       <c r="O3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>38.4</v>
+      </c>
+      <c r="S3" s="6">
+        <f>R3+10</f>
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>32517</v>
       </c>
@@ -617,7 +667,8 @@
       <c r="F4" s="2">
         <v>3.7</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G67" si="0">R4*10</f>
         <v>305</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -644,8 +695,18 @@
       <c r="O4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>30.5</v>
+      </c>
+      <c r="S4" s="6">
+        <f t="shared" ref="S4:S67" si="1">R4+10</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40465</v>
       </c>
@@ -664,7 +725,8 @@
       <c r="F5" s="2">
         <v>12.5</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
         <v>445</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -691,8 +753,21 @@
       <c r="O5" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5">
+        <v>44.5</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" si="1"/>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>50272</v>
       </c>
@@ -711,7 +786,8 @@
       <c r="F6" s="2">
         <v>19.3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
         <v>651</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -738,8 +814,18 @@
       <c r="O6" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="S6" s="6">
+        <f t="shared" si="1"/>
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>50525</v>
       </c>
@@ -758,7 +844,8 @@
       <c r="F7" s="2">
         <v>7.4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
         <v>518</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -785,8 +872,18 @@
       <c r="O7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>51.8</v>
+      </c>
+      <c r="S7" s="6">
+        <f t="shared" si="1"/>
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>50562</v>
       </c>
@@ -805,7 +902,8 @@
       <c r="F8" s="2">
         <v>12.5</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
         <v>688</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -832,8 +930,18 @@
       <c r="O8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>68.8</v>
+      </c>
+      <c r="S8" s="6">
+        <f t="shared" si="1"/>
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>50622</v>
       </c>
@@ -852,7 +960,8 @@
       <c r="F9" s="2">
         <v>9.4</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
         <v>655</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -879,8 +988,18 @@
       <c r="O9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>65.5</v>
+      </c>
+      <c r="S9" s="6">
+        <f t="shared" si="1"/>
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>50646</v>
       </c>
@@ -899,7 +1018,8 @@
       <c r="F10" s="2">
         <v>9.4</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -926,8 +1046,18 @@
       <c r="O10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="S10" s="6">
+        <f t="shared" si="1"/>
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>52344</v>
       </c>
@@ -946,7 +1076,8 @@
       <c r="F11" s="2">
         <v>5.9</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -973,8 +1104,18 @@
       <c r="O11" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>27</v>
+      </c>
+      <c r="S11" s="6">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>60410</v>
       </c>
@@ -993,7 +1134,8 @@
       <c r="F12" s="2">
         <v>15.7</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
         <v>469</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1020,8 +1162,18 @@
       <c r="O12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>46.9</v>
+      </c>
+      <c r="S12" s="6">
+        <f t="shared" si="1"/>
+        <v>56.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>60428</v>
       </c>
@@ -1040,7 +1192,8 @@
       <c r="F13" s="2">
         <v>12</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
         <v>434</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -1067,8 +1220,18 @@
       <c r="O13" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>43.4</v>
+      </c>
+      <c r="S13" s="6">
+        <f t="shared" si="1"/>
+        <v>53.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>60548</v>
       </c>
@@ -1087,7 +1250,8 @@
       <c r="F14" s="2">
         <v>2.1</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1114,8 +1278,18 @@
       <c r="O14" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>43.3</v>
+      </c>
+      <c r="S14" s="6">
+        <f t="shared" si="1"/>
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>62114</v>
       </c>
@@ -1134,7 +1308,8 @@
       <c r="F15" s="2">
         <v>12.6</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
         <v>308</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1161,8 +1336,18 @@
       <c r="O15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>30.8</v>
+      </c>
+      <c r="S15" s="6">
+        <f t="shared" si="1"/>
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>62285</v>
       </c>
@@ -1181,7 +1366,8 @@
       <c r="F16" s="2">
         <v>2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
         <v>707</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -1208,8 +1394,18 @@
       <c r="O16" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>70.7</v>
+      </c>
+      <c r="S16" s="6">
+        <f t="shared" si="1"/>
+        <v>80.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>62291</v>
       </c>
@@ -1228,7 +1424,8 @@
       <c r="F17" s="2">
         <v>5.9</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
         <v>497</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -1255,8 +1452,18 @@
       <c r="O17" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>49.7</v>
+      </c>
+      <c r="S17" s="6">
+        <f t="shared" si="1"/>
+        <v>59.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>62300</v>
       </c>
@@ -1275,7 +1482,8 @@
       <c r="F18" s="2">
         <v>17.5</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
         <v>395</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -1302,8 +1510,18 @@
       <c r="O18" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>39.5</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="1"/>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>70146</v>
       </c>
@@ -1322,7 +1540,8 @@
       <c r="F19" s="2">
         <v>7.2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
         <v>666</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -1349,8 +1568,18 @@
       <c r="O19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="S19" s="6">
+        <f t="shared" si="1"/>
+        <v>76.599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>72104</v>
       </c>
@@ -1369,7 +1598,8 @@
       <c r="F20" s="2">
         <v>17.8</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
         <v>259</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1396,8 +1626,21 @@
       <c r="O20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R20">
+        <v>25.9</v>
+      </c>
+      <c r="S20" s="6">
+        <f t="shared" si="1"/>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>72173</v>
       </c>
@@ -1416,7 +1659,8 @@
       <c r="F21" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
         <v>467</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1443,8 +1687,18 @@
       <c r="O21" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>46.7</v>
+      </c>
+      <c r="S21" s="6">
+        <f t="shared" si="1"/>
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>72228</v>
       </c>
@@ -1463,7 +1717,8 @@
       <c r="F22" s="2">
         <v>6.4</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
         <v>675</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -1490,8 +1745,18 @@
       <c r="O22" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>67.5</v>
+      </c>
+      <c r="S22" s="6">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>72230</v>
       </c>
@@ -1510,7 +1775,8 @@
       <c r="F23" s="2">
         <v>3.3</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
         <v>420</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -1537,8 +1803,21 @@
       <c r="O23" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23">
+        <v>42</v>
+      </c>
+      <c r="S23" s="6">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>80015</v>
       </c>
@@ -1557,7 +1836,8 @@
       <c r="F24" s="2">
         <v>9.9</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
         <v>570</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1584,8 +1864,21 @@
       <c r="O24" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>31</v>
+      </c>
+      <c r="R24">
+        <v>57</v>
+      </c>
+      <c r="S24" s="6">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>80121</v>
       </c>
@@ -1604,7 +1897,8 @@
       <c r="F25" s="2">
         <v>19.2</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -1631,8 +1925,21 @@
       <c r="O25" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>31</v>
+      </c>
+      <c r="R25">
+        <v>11.2</v>
+      </c>
+      <c r="S25" s="6">
+        <f t="shared" si="1"/>
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>82158</v>
       </c>
@@ -1651,7 +1958,8 @@
       <c r="F26" s="2">
         <v>16.3</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
         <v>657</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -1678,8 +1986,18 @@
       <c r="O26" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>65.7</v>
+      </c>
+      <c r="S26" s="6">
+        <f t="shared" si="1"/>
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>82263</v>
       </c>
@@ -1698,7 +2016,8 @@
       <c r="F27" s="2">
         <v>2.4</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
         <v>583</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1725,8 +2044,18 @@
       <c r="O27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>58.3</v>
+      </c>
+      <c r="S27" s="6">
+        <f t="shared" si="1"/>
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>90640</v>
       </c>
@@ -1745,7 +2074,8 @@
       <c r="F28" s="2">
         <v>7.5</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
         <v>458</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -1772,8 +2102,18 @@
       <c r="O28" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>45.8</v>
+      </c>
+      <c r="S28" s="6">
+        <f t="shared" si="1"/>
+        <v>55.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>92016</v>
       </c>
@@ -1792,7 +2132,8 @@
       <c r="F29" s="2">
         <v>3.4</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
         <v>680</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -1819,8 +2160,18 @@
       <c r="O29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>68</v>
+      </c>
+      <c r="S29" s="6">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>92347</v>
       </c>
@@ -1839,7 +2190,8 @@
       <c r="F30" s="2">
         <v>14.5</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
         <v>569</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1866,8 +2218,18 @@
       <c r="O30" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>56.9</v>
+      </c>
+      <c r="S30" s="6">
+        <f t="shared" si="1"/>
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>100955</v>
       </c>
@@ -1886,7 +2248,8 @@
       <c r="F31" s="2">
         <v>6.8</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
         <v>316</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -1913,8 +2276,18 @@
       <c r="O31" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>31.6</v>
+      </c>
+      <c r="S31" s="6">
+        <f t="shared" si="1"/>
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>101192</v>
       </c>
@@ -1933,7 +2306,8 @@
       <c r="F32" s="2">
         <v>3.1</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
+        <f t="shared" si="0"/>
         <v>624</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -1960,8 +2334,18 @@
       <c r="O32" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>62.4</v>
+      </c>
+      <c r="S32" s="6">
+        <f t="shared" si="1"/>
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>101223</v>
       </c>
@@ -1980,7 +2364,8 @@
       <c r="F33" s="2">
         <v>17.8</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
         <v>679</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -2007,8 +2392,21 @@
       <c r="O33" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>31</v>
+      </c>
+      <c r="R33">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="S33" s="6">
+        <f t="shared" si="1"/>
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>102199</v>
       </c>
@@ -2027,7 +2425,8 @@
       <c r="F34" s="2">
         <v>8</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
         <v>442</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -2054,8 +2453,18 @@
       <c r="O34" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>44.2</v>
+      </c>
+      <c r="S34" s="6">
+        <f t="shared" si="1"/>
+        <v>54.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>102313</v>
       </c>
@@ -2074,7 +2483,8 @@
       <c r="F35" s="2">
         <v>1.8</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
+        <f t="shared" si="0"/>
         <v>733</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -2101,8 +2511,21 @@
       <c r="O35" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>31</v>
+      </c>
+      <c r="R35">
+        <v>73.3</v>
+      </c>
+      <c r="S35" s="6">
+        <f t="shared" si="1"/>
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>102423</v>
       </c>
@@ -2121,7 +2544,8 @@
       <c r="F36" s="2">
         <v>1.7</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
+        <f t="shared" si="0"/>
         <v>684</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -2148,8 +2572,18 @@
       <c r="O36" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="S36" s="6">
+        <f t="shared" si="1"/>
+        <v>78.400000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>111217</v>
       </c>
@@ -2168,7 +2602,8 @@
       <c r="F37" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="1">
+        <f t="shared" si="0"/>
         <v>770</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -2195,8 +2630,18 @@
       <c r="O37" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>77</v>
+      </c>
+      <c r="S37" s="6">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>121199</v>
       </c>
@@ -2215,7 +2660,8 @@
       <c r="F38" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
+        <f t="shared" si="0"/>
         <v>415</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -2242,8 +2688,18 @@
       <c r="O38" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>41.5</v>
+      </c>
+      <c r="S38" s="6">
+        <f t="shared" si="1"/>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>122073</v>
       </c>
@@ -2262,7 +2718,8 @@
       <c r="F39" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
+        <f t="shared" si="0"/>
         <v>397</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -2289,8 +2746,18 @@
       <c r="O39" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="S39" s="6">
+        <f t="shared" si="1"/>
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>122140</v>
       </c>
@@ -2309,7 +2776,8 @@
       <c r="F40" s="2">
         <v>9.9</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
+        <f t="shared" si="0"/>
         <v>504</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -2336,8 +2804,18 @@
       <c r="O40" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>50.4</v>
+      </c>
+      <c r="S40" s="6">
+        <f t="shared" si="1"/>
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>122201</v>
       </c>
@@ -2356,7 +2834,8 @@
       <c r="F41" s="2">
         <v>6</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
+        <f t="shared" si="0"/>
         <v>662</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -2383,8 +2862,18 @@
       <c r="O41" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>66.2</v>
+      </c>
+      <c r="S41" s="6">
+        <f t="shared" si="1"/>
+        <v>76.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>122484</v>
       </c>
@@ -2403,7 +2892,8 @@
       <c r="F42" s="2">
         <v>13</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
+        <f t="shared" si="0"/>
         <v>727</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -2430,8 +2920,21 @@
       <c r="O42" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>31</v>
+      </c>
+      <c r="R42">
+        <v>72.7</v>
+      </c>
+      <c r="S42" s="6">
+        <f t="shared" si="1"/>
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>132240</v>
       </c>
@@ -2450,7 +2953,8 @@
       <c r="F43" s="2">
         <v>18.7</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
         <v>392</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -2477,8 +2981,18 @@
       <c r="O43" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="S43" s="6">
+        <f t="shared" si="1"/>
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>132280</v>
       </c>
@@ -2497,7 +3011,8 @@
       <c r="F44" s="2">
         <v>18.2</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -2524,8 +3039,18 @@
       <c r="O44" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>10.3</v>
+      </c>
+      <c r="S44" s="6">
+        <f t="shared" si="1"/>
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>142399</v>
       </c>
@@ -2544,7 +3069,8 @@
       <c r="F45" s="2">
         <v>0.5</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
+        <f t="shared" si="0"/>
         <v>635</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -2571,8 +3097,18 @@
       <c r="O45" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>63.5</v>
+      </c>
+      <c r="S45" s="6">
+        <f t="shared" si="1"/>
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>142520</v>
       </c>
@@ -2591,7 +3127,8 @@
       <c r="F46" s="2">
         <v>9.6</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
+        <f t="shared" si="0"/>
         <v>445</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -2618,8 +3155,18 @@
       <c r="O46" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>44.5</v>
+      </c>
+      <c r="S46" s="6">
+        <f t="shared" si="1"/>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>142548</v>
       </c>
@@ -2638,7 +3185,8 @@
       <c r="F47" s="2">
         <v>4.7</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
+        <f t="shared" si="0"/>
         <v>622</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -2665,8 +3213,18 @@
       <c r="O47" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>62.2</v>
+      </c>
+      <c r="S47" s="6">
+        <f t="shared" si="1"/>
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>152508</v>
       </c>
@@ -2685,7 +3243,8 @@
       <c r="F48" s="2">
         <v>12.4</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
+        <f t="shared" si="0"/>
         <v>492</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -2712,8 +3271,18 @@
       <c r="O48" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>49.2</v>
+      </c>
+      <c r="S48" s="6">
+        <f t="shared" si="1"/>
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>152513</v>
       </c>
@@ -2732,7 +3301,8 @@
       <c r="F49" s="2">
         <v>19.2</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
+        <f t="shared" si="0"/>
         <v>619</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -2759,8 +3329,18 @@
       <c r="O49" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>61.9</v>
+      </c>
+      <c r="S49" s="6">
+        <f t="shared" si="1"/>
+        <v>71.900000000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>160795</v>
       </c>
@@ -2779,7 +3359,8 @@
       <c r="F50" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="1">
+        <f t="shared" si="0"/>
         <v>534</v>
       </c>
       <c r="H50" s="1" t="s">
@@ -2806,8 +3387,18 @@
       <c r="O50" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>53.4</v>
+      </c>
+      <c r="S50" s="6">
+        <f t="shared" si="1"/>
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>161578</v>
       </c>
@@ -2826,7 +3417,8 @@
       <c r="F51" s="2">
         <v>14.7</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="1">
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -2853,8 +3445,18 @@
       <c r="O51" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="R51">
+        <v>22.9</v>
+      </c>
+      <c r="S51" s="6">
+        <f t="shared" si="1"/>
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>162032</v>
       </c>
@@ -2873,7 +3475,8 @@
       <c r="F52" s="2">
         <v>14.6</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="1">
+        <f t="shared" si="0"/>
         <v>530</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -2900,8 +3503,18 @@
       <c r="O52" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>53</v>
+      </c>
+      <c r="S52" s="6">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>162446</v>
       </c>
@@ -2920,7 +3533,8 @@
       <c r="F53" s="2">
         <v>2.9</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="1">
+        <f t="shared" si="0"/>
         <v>805</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -2947,8 +3561,18 @@
       <c r="O53" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>80.5</v>
+      </c>
+      <c r="S53" s="6">
+        <f t="shared" si="1"/>
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>162541</v>
       </c>
@@ -2967,7 +3591,8 @@
       <c r="F54" s="2">
         <v>15.4</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="1">
+        <f t="shared" si="0"/>
         <v>411</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -2994,8 +3619,18 @@
       <c r="O54" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>41.1</v>
+      </c>
+      <c r="S54" s="6">
+        <f t="shared" si="1"/>
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>172162</v>
       </c>
@@ -3014,7 +3649,8 @@
       <c r="F55" s="2">
         <v>8.6</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="1">
+        <f t="shared" si="0"/>
         <v>468</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -3041,8 +3677,21 @@
       <c r="O55" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>31</v>
+      </c>
+      <c r="R55">
+        <v>46.8</v>
+      </c>
+      <c r="S55" s="6">
+        <f t="shared" si="1"/>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>180791</v>
       </c>
@@ -3061,7 +3710,8 @@
       <c r="F56" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="1">
+        <f t="shared" si="0"/>
         <v>404</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -3088,8 +3738,18 @@
       <c r="O56" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>40.4</v>
+      </c>
+      <c r="S56" s="6">
+        <f t="shared" si="1"/>
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>180931</v>
       </c>
@@ -3108,7 +3768,8 @@
       <c r="F57" s="2">
         <v>19.399999999999999</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="1">
+        <f t="shared" si="0"/>
         <v>793</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -3135,8 +3796,18 @@
       <c r="O57" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>79.3</v>
+      </c>
+      <c r="S57" s="6">
+        <f t="shared" si="1"/>
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>180999</v>
       </c>
@@ -3155,7 +3826,8 @@
       <c r="F58" s="2">
         <v>18</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="1">
+        <f t="shared" si="0"/>
         <v>597</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -3182,8 +3854,18 @@
       <c r="O58" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>59.7</v>
+      </c>
+      <c r="S58" s="6">
+        <f t="shared" si="1"/>
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>182050</v>
       </c>
@@ -3202,7 +3884,8 @@
       <c r="F59" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="1">
+        <f t="shared" si="0"/>
         <v>622</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -3229,8 +3912,18 @@
       <c r="O59" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>62.2</v>
+      </c>
+      <c r="S59" s="6">
+        <f t="shared" si="1"/>
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>182085</v>
       </c>
@@ -3249,7 +3942,8 @@
       <c r="F60" s="2">
         <v>1</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
+        <f t="shared" si="0"/>
         <v>468</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -3276,8 +3970,18 @@
       <c r="O60" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <v>46.8</v>
+      </c>
+      <c r="S60" s="6">
+        <f t="shared" si="1"/>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>182310</v>
       </c>
@@ -3296,7 +4000,8 @@
       <c r="F61" s="2">
         <v>13.5</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
+        <f t="shared" si="0"/>
         <v>403</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -3323,8 +4028,18 @@
       <c r="O61" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="S61" s="6">
+        <f t="shared" si="1"/>
+        <v>50.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>182755</v>
       </c>
@@ -3343,7 +4058,8 @@
       <c r="F62" s="2">
         <v>14.3</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
+        <f t="shared" si="0"/>
         <v>780</v>
       </c>
       <c r="H62" s="1" t="s">
@@ -3370,8 +4086,18 @@
       <c r="O62" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>78</v>
+      </c>
+      <c r="S62" s="6">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>192051</v>
       </c>
@@ -3390,7 +4116,8 @@
       <c r="F63" s="2">
         <v>10.8</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
+        <f t="shared" si="0"/>
         <v>136</v>
       </c>
       <c r="H63" s="1" t="s">
@@ -3417,8 +4144,18 @@
       <c r="O63" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>13.6</v>
+      </c>
+      <c r="S63" s="6">
+        <f t="shared" si="1"/>
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>192192</v>
       </c>
@@ -3437,7 +4174,8 @@
       <c r="F64" s="2">
         <v>2.4</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
+        <f t="shared" si="0"/>
         <v>570</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -3464,8 +4202,18 @@
       <c r="O64" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>57</v>
+      </c>
+      <c r="S64" s="6">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>192246</v>
       </c>
@@ -3484,7 +4232,8 @@
       <c r="F65" s="2">
         <v>1</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
+        <f t="shared" si="0"/>
         <v>386</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -3511,8 +4260,18 @@
       <c r="O65" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>38.6</v>
+      </c>
+      <c r="S65" s="6">
+        <f t="shared" si="1"/>
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>201331</v>
       </c>
@@ -3531,7 +4290,8 @@
       <c r="F66" s="2">
         <v>9.5</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
+        <f t="shared" si="0"/>
         <v>437</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -3558,8 +4318,18 @@
       <c r="O66" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>43.7</v>
+      </c>
+      <c r="S66" s="6">
+        <f t="shared" si="1"/>
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>202004</v>
       </c>
@@ -3578,7 +4348,8 @@
       <c r="F67" s="2">
         <v>2.7</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
+        <f t="shared" si="0"/>
         <v>454</v>
       </c>
       <c r="H67" s="1" t="s">
@@ -3605,8 +4376,18 @@
       <c r="O67" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>45.4</v>
+      </c>
+      <c r="S67" s="6">
+        <f t="shared" si="1"/>
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>202965</v>
       </c>
@@ -3625,7 +4406,8 @@
       <c r="F68" s="2">
         <v>16.3</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
+        <f t="shared" ref="G68" si="2">R68*10</f>
         <v>445</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -3652,12 +4434,455 @@
       <c r="O68" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="P68">
+        <v>1</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>31</v>
+      </c>
+      <c r="R68">
+        <v>44.5</v>
+      </c>
+      <c r="S68" s="6">
+        <f t="shared" ref="S68" si="3">R68+10</f>
+        <v>54.5</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S68">
+    <filterColumn colId="0" showButton="0"/>
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="5" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="13" showButton="0"/>
+  </autoFilter>
+  <sortState ref="S3:S68">
+    <sortCondition ref="S3"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:D66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="6">
+        <f>Sheet1!R44+10</f>
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6">
+        <f>Sheet1!R25+10</f>
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6">
+        <f>Sheet1!R63+10</f>
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="6">
+        <f>Sheet1!R51+10</f>
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="6">
+        <f>Sheet1!R20+10</f>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="6">
+        <f>Sheet1!R11+10</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="6">
+        <f>Sheet1!R4+10</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="6">
+        <f>Sheet1!R15+10</f>
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="6">
+        <f>Sheet1!R31+10</f>
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="6">
+        <f>Sheet1!R10+10</f>
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="6">
+        <f>Sheet1!R3+10</f>
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="6">
+        <f>Sheet1!R65+10</f>
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="6">
+        <f>Sheet1!R43+10</f>
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="6">
+        <f>Sheet1!R18+10</f>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="6">
+        <f>Sheet1!R39+10</f>
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="6">
+        <f>Sheet1!R61+10</f>
+        <v>50.3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="6">
+        <f>Sheet1!R56+10</f>
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="6">
+        <f>Sheet1!R54+10</f>
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="6">
+        <f>Sheet1!R38+10</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="6">
+        <f>Sheet1!R23+10</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="6">
+        <f>Sheet1!R14+10</f>
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="6">
+        <f>Sheet1!R13+10</f>
+        <v>53.4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="6">
+        <f>Sheet1!R66+10</f>
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="6">
+        <f>Sheet1!R34+10</f>
+        <v>54.2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="6">
+        <f>Sheet1!R5+10</f>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="6">
+        <f>Sheet1!R46+10</f>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="6">
+        <f>Sheet1!R68+10</f>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="6">
+        <f>Sheet1!R67+10</f>
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="6">
+        <f>Sheet1!R28+10</f>
+        <v>55.8</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="6">
+        <f>Sheet1!R21+10</f>
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="6">
+        <f>Sheet1!R55+10</f>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="6">
+        <f>Sheet1!R60+10</f>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="6">
+        <f>Sheet1!R12+10</f>
+        <v>56.9</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="6">
+        <f>Sheet1!R48+10</f>
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="6">
+        <f>Sheet1!R17+10</f>
+        <v>59.7</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="6">
+        <f>Sheet1!R40+10</f>
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="6">
+        <f>Sheet1!R7+10</f>
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="6">
+        <f>Sheet1!R52+10</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="6">
+        <f>Sheet1!R50+10</f>
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="6">
+        <f>Sheet1!R30+10</f>
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="6">
+        <f>Sheet1!R24+10</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="6">
+        <f>Sheet1!R64+10</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="6">
+        <f>Sheet1!R27+10</f>
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="6">
+        <f>Sheet1!R58+10</f>
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="6">
+        <f>Sheet1!R49+10</f>
+        <v>71.900000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="6">
+        <f>Sheet1!R47+10</f>
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="6">
+        <f>Sheet1!R59+10</f>
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="6">
+        <f>Sheet1!R32+10</f>
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="6">
+        <f>Sheet1!R45+10</f>
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="6">
+        <f>Sheet1!R6+10</f>
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="6">
+        <f>Sheet1!R9+10</f>
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="6">
+        <f>Sheet1!R26+10</f>
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="6">
+        <f>Sheet1!R41+10</f>
+        <v>76.2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="6">
+        <f>Sheet1!R19+10</f>
+        <v>76.599999999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="6">
+        <f>Sheet1!R22+10</f>
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="6">
+        <f>Sheet1!R33+10</f>
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="6">
+        <f>Sheet1!R29+10</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="6">
+        <f>Sheet1!R36+10</f>
+        <v>78.400000000000006</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="6">
+        <f>Sheet1!R8+10</f>
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="6">
+        <f>Sheet1!R16+10</f>
+        <v>80.7</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="6">
+        <f>Sheet1!R42+10</f>
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="6">
+        <f>Sheet1!R35+10</f>
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="6">
+        <f>Sheet1!R37+10</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="6">
+        <f>Sheet1!R62+10</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="6">
+        <f>Sheet1!R57+10</f>
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="6">
+        <f>Sheet1!R53+10</f>
+        <v>90.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>